<commit_message>
stec os + rein
</commit_message>
<xml_diff>
--- a/Plancheck/plancheck_data/check_protocol/STEC Os 5F.xlsx
+++ b/Plancheck/plancheck_data/check_protocol/STEC Os 5F.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5400" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5400" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="General data" sheetId="1" r:id="rId1"/>
@@ -412,9 +412,6 @@
     <t>ParoiThoracique</t>
   </si>
   <si>
-    <t>D0,5cc&lt;39gy</t>
-  </si>
-  <si>
     <t>V32Gy&lt;30cc</t>
   </si>
   <si>
@@ -484,9 +481,6 @@
     <t>Canal Med</t>
   </si>
   <si>
-    <t>Tron Cerebral</t>
-  </si>
-  <si>
     <t>D0,5cc&lt;32Gy</t>
   </si>
   <si>
@@ -530,6 +524,12 @@
   </si>
   <si>
     <t>D0,5cc&lt;53Gy</t>
+  </si>
+  <si>
+    <t>D0,5cc&lt;39Gy</t>
+  </si>
+  <si>
+    <t>Tronc Cerebral</t>
   </si>
 </sst>
 </file>
@@ -1524,7 +1524,7 @@
   </sheetPr>
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
@@ -2350,7 +2350,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:C8"/>
+      <selection activeCell="D1" sqref="D1:AD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2402,10 +2402,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="A8" sqref="A8:XFD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2463,9 +2463,6 @@
       <c r="A7" s="11" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2480,7 +2477,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A6" sqref="A6:XFD53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2555,8 +2552,8 @@
   </sheetPr>
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2656,10 +2653,10 @@
         <v>128</v>
       </c>
       <c r="B7" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="C7" s="33" t="s">
         <v>129</v>
-      </c>
-      <c r="C7" s="33" t="s">
-        <v>130</v>
       </c>
       <c r="D7" s="33"/>
       <c r="E7" s="33"/>
@@ -2667,10 +2664,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C8" s="33"/>
       <c r="D8" s="33"/>
@@ -2679,10 +2676,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C9" s="33"/>
       <c r="D9" s="33"/>
@@ -2691,10 +2688,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B10" s="33" t="s">
         <v>133</v>
-      </c>
-      <c r="B10" s="33" t="s">
-        <v>134</v>
       </c>
       <c r="C10" s="33"/>
       <c r="D10" s="33"/>
@@ -2703,53 +2700,53 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B11" s="33" t="s">
         <v>124</v>
       </c>
       <c r="C11" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="D11" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="D11" s="33" t="s">
+      <c r="E11" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="E11" s="33" t="s">
+      <c r="F11" s="33" t="s">
         <v>138</v>
-      </c>
-      <c r="F11" s="33" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B12" s="33" t="s">
         <v>124</v>
       </c>
       <c r="C12" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="D12" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="D12" s="33" t="s">
+      <c r="E12" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="E12" s="33" t="s">
+      <c r="F12" s="33" t="s">
         <v>138</v>
-      </c>
-      <c r="F12" s="33" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B13" s="33" t="s">
         <v>124</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D13" s="33"/>
       <c r="E13" s="33"/>
@@ -2757,10 +2754,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B14" s="33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C14" s="33"/>
       <c r="D14" s="33"/>
@@ -2769,10 +2766,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B15" s="33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C15" s="33"/>
       <c r="D15" s="33"/>
@@ -2781,10 +2778,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C16" s="33"/>
       <c r="D16" s="33"/>
@@ -2793,13 +2790,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D17" s="33"/>
       <c r="E17" s="33"/>
@@ -2807,13 +2804,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B18" s="33" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C18" s="33" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D18" s="33"/>
       <c r="E18" s="33"/>
@@ -2821,10 +2818,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C19" s="33"/>
       <c r="D19" s="33"/>
@@ -2833,10 +2830,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B20" s="33" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C20" s="33"/>
       <c r="D20" s="33"/>
@@ -2845,10 +2842,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B21" s="33" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C21" s="33"/>
       <c r="D21" s="33"/>
@@ -2857,13 +2854,13 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B22" s="33" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C22" s="33" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D22" s="33"/>
       <c r="E22" s="33"/>
@@ -2871,13 +2868,13 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B23" s="33" t="s">
         <v>118</v>
       </c>
       <c r="C23" s="33" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D23" s="33"/>
       <c r="E23" s="33"/>
@@ -2885,13 +2882,13 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>153</v>
+        <v>168</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C24" s="33" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D24" s="33"/>
       <c r="E24" s="33"/>
@@ -2899,10 +2896,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B25" s="33" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C25" s="33"/>
       <c r="D25" s="33"/>
@@ -2911,10 +2908,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B26" s="33" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C26" s="33"/>
       <c r="D26" s="33"/>
@@ -2923,13 +2920,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B27" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="C27" s="33" t="s">
         <v>158</v>
-      </c>
-      <c r="B27" s="33" t="s">
-        <v>159</v>
-      </c>
-      <c r="C27" s="33" t="s">
-        <v>160</v>
       </c>
       <c r="D27" s="33"/>
       <c r="E27" s="33"/>

</xml_diff>